<commit_message>
[fix]: obligatory individual project subject
</commit_message>
<xml_diff>
--- a/src/extraResources/plan-templates/table.xlsx
+++ b/src/extraResources/plan-templates/table.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="УП НОО (1-4 классы)" sheetId="3" r:id="rId1"/>
@@ -779,7 +779,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1003,6 +1003,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1012,17 +1015,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1036,19 +1051,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1333,7 +1336,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="81" zoomScaleNormal="81" workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -1430,7 +1433,7 @@
       <c r="I5" s="27"/>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="85" t="s">
         <v>122</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1447,7 +1450,7 @@
       <c r="I6" s="27"/>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
+      <c r="A7" s="85"/>
       <c r="B7" s="8" t="s">
         <v>123</v>
       </c>
@@ -1462,7 +1465,7 @@
       <c r="I7" s="27"/>
     </row>
     <row r="8" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="85" t="s">
         <v>124</v>
       </c>
       <c r="B8" s="8" t="s">
@@ -1479,7 +1482,7 @@
       <c r="I8" s="27"/>
     </row>
     <row r="9" spans="1:64" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
+      <c r="A9" s="85"/>
       <c r="B9" s="8" t="s">
         <v>125</v>
       </c>
@@ -1545,7 +1548,7 @@
       <c r="I12" s="27"/>
     </row>
     <row r="13" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="88" t="s">
+      <c r="A13" s="85" t="s">
         <v>129</v>
       </c>
       <c r="B13" s="8" t="s">
@@ -1562,7 +1565,7 @@
       <c r="I13" s="27"/>
     </row>
     <row r="14" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="88"/>
+      <c r="A14" s="85"/>
       <c r="B14" s="8" t="s">
         <v>130</v>
       </c>
@@ -1575,7 +1578,7 @@
       <c r="I14" s="27"/>
     </row>
     <row r="15" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
+      <c r="A15" s="85"/>
       <c r="B15" s="8" t="s">
         <v>131</v>
       </c>
@@ -1588,7 +1591,7 @@
       <c r="I15" s="27"/>
     </row>
     <row r="16" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="88"/>
+      <c r="A16" s="85"/>
       <c r="B16" s="8" t="s">
         <v>132</v>
       </c>
@@ -1656,7 +1659,7 @@
       <c r="BL16" s="69"/>
     </row>
     <row r="17" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="88"/>
+      <c r="A17" s="85"/>
       <c r="B17" s="8" t="s">
         <v>133</v>
       </c>
@@ -1724,7 +1727,7 @@
       <c r="BL17" s="69"/>
     </row>
     <row r="18" spans="1:64" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="88"/>
+      <c r="A18" s="85"/>
       <c r="B18" s="8" t="s">
         <v>134</v>
       </c>
@@ -1792,7 +1795,7 @@
       <c r="BL18" s="69"/>
     </row>
     <row r="19" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="88"/>
+      <c r="A19" s="85"/>
       <c r="B19" s="8" t="s">
         <v>135</v>
       </c>
@@ -1860,7 +1863,7 @@
       <c r="BL19" s="69"/>
     </row>
     <row r="20" spans="1:64" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="88" t="s">
+      <c r="A20" s="85" t="s">
         <v>105</v>
       </c>
       <c r="B20" s="8" t="s">
@@ -1932,7 +1935,7 @@
       <c r="BL20" s="69"/>
     </row>
     <row r="21" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A21" s="88"/>
+      <c r="A21" s="85"/>
       <c r="B21" s="8" t="s">
         <v>107</v>
       </c>
@@ -2484,7 +2487,7 @@
       <c r="BL28" s="69"/>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A29" s="85" t="s">
+      <c r="A29" s="86" t="s">
         <v>119</v>
       </c>
       <c r="B29" s="80" t="s">
@@ -2556,7 +2559,7 @@
       <c r="BL29" s="69"/>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A30" s="85"/>
+      <c r="A30" s="86"/>
       <c r="B30" s="80">
         <v>2954</v>
       </c>
@@ -2626,7 +2629,7 @@
       <c r="BL30" s="69"/>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A31" s="86" t="s">
+      <c r="A31" s="87" t="s">
         <v>118</v>
       </c>
       <c r="B31" s="80">
@@ -2702,7 +2705,7 @@
       <c r="BL31" s="69"/>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A32" s="87"/>
+      <c r="A32" s="88"/>
       <c r="B32" s="80">
         <v>21</v>
       </c>
@@ -3277,8 +3280,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL60"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView zoomScale="54" zoomScaleNormal="54" workbookViewId="0">
+      <selection activeCell="X12" sqref="X12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3542,7 +3545,7 @@
       <c r="AB5" s="44"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="85" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -3584,7 +3587,7 @@
       <c r="AB6" s="44"/>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
+      <c r="A7" s="85"/>
       <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
@@ -3618,7 +3621,7 @@
       <c r="AB7" s="44"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="85" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="6" t="s">
@@ -3654,7 +3657,7 @@
       <c r="AB8" s="44"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
+      <c r="A9" s="85"/>
       <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
@@ -3688,7 +3691,7 @@
       <c r="AB9" s="44"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="85" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -3730,7 +3733,7 @@
       <c r="AB10" s="44"/>
     </row>
     <row r="11" spans="1:28" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="88"/>
+      <c r="A11" s="85"/>
       <c r="B11" s="6" t="s">
         <v>19</v>
       </c>
@@ -3770,7 +3773,7 @@
       <c r="AB11" s="44"/>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="85" t="s">
         <v>28</v>
       </c>
       <c r="B12" s="6" t="s">
@@ -3818,7 +3821,7 @@
       <c r="AB12" s="44"/>
     </row>
     <row r="13" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A13" s="88"/>
+      <c r="A13" s="85"/>
       <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
@@ -3858,7 +3861,7 @@
       <c r="AB13" s="44"/>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A14" s="88" t="s">
+      <c r="A14" s="85" t="s">
         <v>99</v>
       </c>
       <c r="B14" s="6" t="s">
@@ -3894,7 +3897,7 @@
       <c r="AB14" s="44"/>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
+      <c r="A15" s="85"/>
       <c r="B15" s="6" t="s">
         <v>25</v>
       </c>
@@ -3928,7 +3931,7 @@
       <c r="AB15" s="44"/>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.3">
-      <c r="A16" s="88"/>
+      <c r="A16" s="85"/>
       <c r="B16" s="6" t="s">
         <v>22</v>
       </c>
@@ -3962,7 +3965,7 @@
       <c r="AB16" s="44"/>
     </row>
     <row r="17" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A17" s="88" t="s">
+      <c r="A17" s="85" t="s">
         <v>101</v>
       </c>
       <c r="B17" s="6" t="s">
@@ -3998,7 +4001,7 @@
       <c r="AB17" s="44"/>
     </row>
     <row r="18" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A18" s="88"/>
+      <c r="A18" s="85"/>
       <c r="B18" s="6" t="s">
         <v>102</v>
       </c>
@@ -4038,7 +4041,7 @@
       <c r="AB18" s="44"/>
     </row>
     <row r="19" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A19" s="88"/>
+      <c r="A19" s="85"/>
       <c r="B19" s="6" t="s">
         <v>37</v>
       </c>
@@ -4114,7 +4117,7 @@
       <c r="AB20" s="44"/>
     </row>
     <row r="21" spans="1:64" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A21" s="88" t="s">
+      <c r="A21" s="85" t="s">
         <v>105</v>
       </c>
       <c r="B21" s="6" t="s">
@@ -4150,7 +4153,7 @@
       <c r="AB21" s="44"/>
     </row>
     <row r="22" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A22" s="88"/>
+      <c r="A22" s="85"/>
       <c r="B22" s="6" t="s">
         <v>107</v>
       </c>
@@ -4226,7 +4229,7 @@
       <c r="AB23" s="44"/>
     </row>
     <row r="24" spans="1:64" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="85" t="s">
         <v>109</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -4262,7 +4265,7 @@
       <c r="AB24" s="44"/>
     </row>
     <row r="25" spans="1:64" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="88"/>
+      <c r="A25" s="85"/>
       <c r="B25" s="6" t="s">
         <v>42</v>
       </c>
@@ -4358,10 +4361,10 @@
       <c r="AB27" s="44"/>
     </row>
     <row r="28" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="89" t="s">
         <v>110</v>
       </c>
-      <c r="B28" s="90"/>
+      <c r="B28" s="89"/>
       <c r="C28" s="61"/>
       <c r="D28" s="18"/>
       <c r="E28" s="18"/>
@@ -4371,10 +4374,10 @@
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
-      <c r="L28" s="89">
+      <c r="L28" s="91">
         <v>2</v>
       </c>
-      <c r="M28" s="89"/>
+      <c r="M28" s="91"/>
       <c r="N28" s="46"/>
       <c r="O28" s="46"/>
       <c r="P28" s="46"/>
@@ -4392,10 +4395,10 @@
       <c r="AB28" s="44"/>
     </row>
     <row r="29" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A29" s="90" t="s">
+      <c r="A29" s="89" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="90"/>
+      <c r="B29" s="89"/>
       <c r="C29" s="61"/>
       <c r="D29" s="18"/>
       <c r="E29" s="18"/>
@@ -4406,10 +4409,10 @@
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
       <c r="L29" s="18"/>
-      <c r="M29" s="89">
+      <c r="M29" s="91">
         <v>2</v>
       </c>
-      <c r="N29" s="89"/>
+      <c r="N29" s="91"/>
       <c r="O29" s="46"/>
       <c r="P29" s="46"/>
       <c r="Q29" s="46"/>
@@ -4426,10 +4429,10 @@
       <c r="AB29" s="44"/>
     </row>
     <row r="30" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A30" s="90" t="s">
+      <c r="A30" s="89" t="s">
         <v>112</v>
       </c>
-      <c r="B30" s="90"/>
+      <c r="B30" s="89"/>
       <c r="C30" s="61"/>
       <c r="D30" s="18"/>
       <c r="E30" s="18"/>
@@ -4440,10 +4443,10 @@
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
       <c r="L30" s="18"/>
-      <c r="M30" s="89">
+      <c r="M30" s="91">
         <v>2</v>
       </c>
-      <c r="N30" s="89"/>
+      <c r="N30" s="91"/>
       <c r="O30" s="46"/>
       <c r="P30" s="46"/>
       <c r="Q30" s="46"/>
@@ -4460,10 +4463,10 @@
       <c r="AB30" s="44"/>
     </row>
     <row r="31" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A31" s="90" t="s">
+      <c r="A31" s="89" t="s">
         <v>56</v>
       </c>
-      <c r="B31" s="90"/>
+      <c r="B31" s="89"/>
       <c r="C31" s="61"/>
       <c r="D31" s="18"/>
       <c r="E31" s="18"/>
@@ -4498,10 +4501,10 @@
       <c r="AB31" s="44"/>
     </row>
     <row r="32" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A32" s="90" t="s">
+      <c r="A32" s="89" t="s">
         <v>113</v>
       </c>
-      <c r="B32" s="90"/>
+      <c r="B32" s="89"/>
       <c r="C32" s="61"/>
       <c r="D32" s="18"/>
       <c r="E32" s="18"/>
@@ -4517,11 +4520,11 @@
       <c r="O32" s="46"/>
       <c r="P32" s="46"/>
       <c r="Q32" s="46"/>
-      <c r="R32" s="91">
+      <c r="R32" s="90">
         <v>2</v>
       </c>
-      <c r="S32" s="91"/>
-      <c r="T32" s="91"/>
+      <c r="S32" s="90"/>
+      <c r="T32" s="90"/>
       <c r="U32" s="46"/>
       <c r="V32" s="46"/>
       <c r="W32" s="46"/>
@@ -4568,10 +4571,10 @@
       <c r="BL32" s="64"/>
     </row>
     <row r="33" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A33" s="90" t="s">
+      <c r="A33" s="89" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="90"/>
+      <c r="B33" s="89"/>
       <c r="C33" s="61"/>
       <c r="D33" s="18"/>
       <c r="E33" s="18"/>
@@ -4587,11 +4590,11 @@
       <c r="O33" s="46"/>
       <c r="P33" s="46"/>
       <c r="Q33" s="46"/>
-      <c r="R33" s="91">
+      <c r="R33" s="90">
         <v>2</v>
       </c>
-      <c r="S33" s="91"/>
-      <c r="T33" s="91"/>
+      <c r="S33" s="90"/>
+      <c r="T33" s="90"/>
       <c r="U33" s="46"/>
       <c r="V33" s="46"/>
       <c r="W33" s="46"/>
@@ -4638,10 +4641,10 @@
       <c r="BL33" s="64"/>
     </row>
     <row r="34" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A34" s="90" t="s">
+      <c r="A34" s="89" t="s">
         <v>115</v>
       </c>
-      <c r="B34" s="90"/>
+      <c r="B34" s="89"/>
       <c r="C34" s="61"/>
       <c r="D34" s="18"/>
       <c r="E34" s="18"/>
@@ -4660,10 +4663,10 @@
       <c r="R34" s="46"/>
       <c r="S34" s="46"/>
       <c r="T34" s="46"/>
-      <c r="U34" s="91">
+      <c r="U34" s="90">
         <v>2</v>
       </c>
-      <c r="V34" s="91"/>
+      <c r="V34" s="90"/>
       <c r="W34" s="46"/>
       <c r="X34" s="46"/>
       <c r="Y34" s="46"/>
@@ -4708,10 +4711,10 @@
       <c r="BL34" s="64"/>
     </row>
     <row r="35" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A35" s="90" t="s">
+      <c r="A35" s="89" t="s">
         <v>116</v>
       </c>
-      <c r="B35" s="90"/>
+      <c r="B35" s="89"/>
       <c r="C35" s="61"/>
       <c r="D35" s="18"/>
       <c r="E35" s="18"/>
@@ -4731,10 +4734,10 @@
       <c r="S35" s="46"/>
       <c r="T35" s="46"/>
       <c r="U35" s="46"/>
-      <c r="V35" s="91">
+      <c r="V35" s="90">
         <v>2</v>
       </c>
-      <c r="W35" s="91"/>
+      <c r="W35" s="90"/>
       <c r="X35" s="46"/>
       <c r="Y35" s="46"/>
       <c r="Z35" s="46"/>
@@ -4982,7 +4985,7 @@
       <c r="BL38" s="64"/>
     </row>
     <row r="39" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A39" s="90" t="s">
+      <c r="A39" s="89" t="s">
         <v>119</v>
       </c>
       <c r="B39" s="46" t="s">
@@ -5054,7 +5057,7 @@
       <c r="BL39" s="64"/>
     </row>
     <row r="40" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A40" s="90"/>
+      <c r="A40" s="89"/>
       <c r="B40" s="46">
         <v>5058</v>
       </c>
@@ -5124,7 +5127,7 @@
       <c r="BL40" s="64"/>
     </row>
     <row r="41" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A41" s="86" t="s">
+      <c r="A41" s="87" t="s">
         <v>118</v>
       </c>
       <c r="B41" s="46">
@@ -5202,7 +5205,7 @@
       <c r="BL41" s="64"/>
     </row>
     <row r="42" spans="1:64" x14ac:dyDescent="0.3">
-      <c r="A42" s="87"/>
+      <c r="A42" s="88"/>
       <c r="B42" s="46">
         <v>29</v>
       </c>
@@ -5709,21 +5712,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="R33:T33"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="A30:B30"/>
-    <mergeCell ref="M30:N30"/>
-    <mergeCell ref="A31:B31"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="R32:T32"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="U34:V34"/>
-    <mergeCell ref="A35:B35"/>
-    <mergeCell ref="V35:W35"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="L28:M28"/>
     <mergeCell ref="A29:B29"/>
@@ -5734,6 +5722,21 @@
     <mergeCell ref="A14:A16"/>
     <mergeCell ref="A17:A19"/>
     <mergeCell ref="A21:A22"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="U34:V34"/>
+    <mergeCell ref="A35:B35"/>
+    <mergeCell ref="V35:W35"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="R33:T33"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="A30:B30"/>
+    <mergeCell ref="M30:N30"/>
+    <mergeCell ref="A31:B31"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="R32:T32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -5744,8 +5747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BI91"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="59" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="AV73" sqref="AV73:AW78"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="59" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AF25" sqref="AF25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5773,20 +5776,20 @@
       <c r="C1" s="27" t="s">
         <v>159</v>
       </c>
-      <c r="D1" s="100"/>
-      <c r="E1" s="100"/>
-      <c r="F1" s="100"/>
-      <c r="G1" s="100"/>
-      <c r="H1" s="100"/>
-      <c r="I1" s="100"/>
-      <c r="J1" s="100"/>
-      <c r="K1" s="100"/>
-      <c r="L1" s="100"/>
-      <c r="M1" s="100"/>
-      <c r="N1" s="96" t="s">
+      <c r="D1" s="94"/>
+      <c r="E1" s="94"/>
+      <c r="F1" s="94"/>
+      <c r="G1" s="94"/>
+      <c r="H1" s="94"/>
+      <c r="I1" s="94"/>
+      <c r="J1" s="94"/>
+      <c r="K1" s="94"/>
+      <c r="L1" s="94"/>
+      <c r="M1" s="94"/>
+      <c r="N1" s="93" t="s">
         <v>155</v>
       </c>
-      <c r="O1" s="96"/>
+      <c r="O1" s="93"/>
       <c r="P1" s="28" t="s">
         <v>141</v>
       </c>
@@ -5829,58 +5832,58 @@
       <c r="AC1" s="28" t="s">
         <v>147</v>
       </c>
-      <c r="AD1" s="96" t="s">
+      <c r="AD1" s="93" t="s">
         <v>148</v>
       </c>
-      <c r="AE1" s="96"/>
-      <c r="AF1" s="96" t="s">
+      <c r="AE1" s="93"/>
+      <c r="AF1" s="93" t="s">
         <v>149</v>
       </c>
-      <c r="AG1" s="96"/>
-      <c r="AH1" s="96" t="s">
+      <c r="AG1" s="93"/>
+      <c r="AH1" s="93" t="s">
         <v>150</v>
       </c>
-      <c r="AI1" s="96"/>
-      <c r="AJ1" s="96" t="s">
+      <c r="AI1" s="93"/>
+      <c r="AJ1" s="93" t="s">
         <v>151</v>
       </c>
-      <c r="AK1" s="96"/>
-      <c r="AL1" s="96" t="s">
+      <c r="AK1" s="93"/>
+      <c r="AL1" s="93" t="s">
         <v>91</v>
       </c>
-      <c r="AM1" s="96"/>
-      <c r="AN1" s="96" t="s">
+      <c r="AM1" s="93"/>
+      <c r="AN1" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="AO1" s="96"/>
-      <c r="AP1" s="96" t="s">
+      <c r="AO1" s="93"/>
+      <c r="AP1" s="93" t="s">
         <v>0</v>
       </c>
-      <c r="AQ1" s="96"/>
-      <c r="AR1" s="96" t="s">
+      <c r="AQ1" s="93"/>
+      <c r="AR1" s="93" t="s">
         <v>153</v>
       </c>
-      <c r="AS1" s="96"/>
-      <c r="AT1" s="96" t="s">
+      <c r="AS1" s="93"/>
+      <c r="AT1" s="93" t="s">
         <v>144</v>
       </c>
-      <c r="AU1" s="96"/>
-      <c r="AV1" s="96" t="s">
-        <v>1</v>
-      </c>
-      <c r="AW1" s="96"/>
-      <c r="AX1" s="96" t="s">
+      <c r="AU1" s="93"/>
+      <c r="AV1" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="AW1" s="93"/>
+      <c r="AX1" s="93" t="s">
         <v>2</v>
       </c>
-      <c r="AY1" s="96"/>
-      <c r="AZ1" s="96" t="s">
+      <c r="AY1" s="93"/>
+      <c r="AZ1" s="93" t="s">
         <v>152</v>
       </c>
-      <c r="BA1" s="96"/>
-      <c r="BB1" s="96" t="s">
+      <c r="BA1" s="93"/>
+      <c r="BB1" s="93" t="s">
         <v>154</v>
       </c>
-      <c r="BC1" s="96"/>
+      <c r="BC1" s="93"/>
       <c r="BD1" s="28" t="s">
         <v>155</v>
       </c>
@@ -6381,7 +6384,7 @@
       <c r="BI5" s="27"/>
     </row>
     <row r="6" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="88" t="s">
+      <c r="A6" s="85" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -6466,7 +6469,7 @@
       <c r="BI6" s="27"/>
     </row>
     <row r="7" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A7" s="88"/>
+      <c r="A7" s="85"/>
       <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
@@ -6545,7 +6548,7 @@
       <c r="BI7" s="27"/>
     </row>
     <row r="8" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A8" s="88" t="s">
+      <c r="A8" s="85" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -6614,7 +6617,7 @@
       <c r="BI8" s="27"/>
     </row>
     <row r="9" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A9" s="88"/>
+      <c r="A9" s="85"/>
       <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
@@ -6681,7 +6684,7 @@
       <c r="BI9" s="27"/>
     </row>
     <row r="10" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A10" s="88" t="s">
+      <c r="A10" s="85" t="s">
         <v>17</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -6766,7 +6769,7 @@
       <c r="BI10" s="27"/>
     </row>
     <row r="11" spans="1:61" ht="60" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="88"/>
+      <c r="A11" s="85"/>
       <c r="B11" s="2" t="s">
         <v>19</v>
       </c>
@@ -6833,7 +6836,7 @@
       <c r="BI11" s="27"/>
     </row>
     <row r="12" spans="1:61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="85" t="s">
         <v>20</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -6842,194 +6845,194 @@
       <c r="C12" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D12" s="92">
-        <v>1</v>
-      </c>
-      <c r="E12" s="93"/>
-      <c r="F12" s="92">
-        <v>1</v>
-      </c>
-      <c r="G12" s="93"/>
-      <c r="H12" s="92">
-        <v>1</v>
-      </c>
-      <c r="I12" s="93"/>
-      <c r="J12" s="92">
-        <v>1</v>
-      </c>
-      <c r="K12" s="93"/>
-      <c r="L12" s="92">
-        <v>1</v>
-      </c>
-      <c r="M12" s="93"/>
-      <c r="N12" s="92">
-        <v>1</v>
-      </c>
-      <c r="O12" s="93"/>
-      <c r="P12" s="92">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="93"/>
-      <c r="R12" s="92">
-        <v>1</v>
-      </c>
-      <c r="S12" s="93"/>
-      <c r="T12" s="92">
-        <v>1</v>
-      </c>
-      <c r="U12" s="93"/>
-      <c r="V12" s="92">
-        <v>1</v>
-      </c>
-      <c r="W12" s="93"/>
-      <c r="X12" s="92">
-        <v>1</v>
-      </c>
-      <c r="Y12" s="93"/>
-      <c r="Z12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AA12" s="93"/>
-      <c r="AB12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AC12" s="93"/>
-      <c r="AD12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AE12" s="93"/>
-      <c r="AF12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AG12" s="93"/>
-      <c r="AH12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AI12" s="93"/>
-      <c r="AJ12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AK12" s="93"/>
-      <c r="AL12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AM12" s="93"/>
+      <c r="D12" s="97">
+        <v>1</v>
+      </c>
+      <c r="E12" s="98"/>
+      <c r="F12" s="97">
+        <v>1</v>
+      </c>
+      <c r="G12" s="98"/>
+      <c r="H12" s="97">
+        <v>1</v>
+      </c>
+      <c r="I12" s="98"/>
+      <c r="J12" s="97">
+        <v>1</v>
+      </c>
+      <c r="K12" s="98"/>
+      <c r="L12" s="97">
+        <v>1</v>
+      </c>
+      <c r="M12" s="98"/>
+      <c r="N12" s="97">
+        <v>1</v>
+      </c>
+      <c r="O12" s="98"/>
+      <c r="P12" s="97">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="98"/>
+      <c r="R12" s="97">
+        <v>1</v>
+      </c>
+      <c r="S12" s="98"/>
+      <c r="T12" s="97">
+        <v>1</v>
+      </c>
+      <c r="U12" s="98"/>
+      <c r="V12" s="97">
+        <v>1</v>
+      </c>
+      <c r="W12" s="98"/>
+      <c r="X12" s="97">
+        <v>1</v>
+      </c>
+      <c r="Y12" s="98"/>
+      <c r="Z12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AA12" s="98"/>
+      <c r="AB12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AC12" s="98"/>
+      <c r="AD12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AE12" s="98"/>
+      <c r="AF12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AG12" s="98"/>
+      <c r="AH12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AI12" s="98"/>
+      <c r="AJ12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AK12" s="98"/>
+      <c r="AL12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AM12" s="98"/>
       <c r="AN12" s="40">
         <v>1</v>
       </c>
       <c r="AO12" s="40">
         <v>1</v>
       </c>
-      <c r="AP12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AQ12" s="93"/>
-      <c r="AR12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AS12" s="93"/>
-      <c r="AT12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AU12" s="93"/>
-      <c r="AV12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AW12" s="93"/>
-      <c r="AX12" s="92">
-        <v>1</v>
-      </c>
-      <c r="AY12" s="93"/>
+      <c r="AP12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AQ12" s="98"/>
+      <c r="AR12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="98"/>
+      <c r="AT12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AU12" s="98"/>
+      <c r="AV12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AW12" s="98"/>
+      <c r="AX12" s="97">
+        <v>1</v>
+      </c>
+      <c r="AY12" s="98"/>
       <c r="AZ12" s="40">
         <v>1</v>
       </c>
       <c r="BA12" s="40">
         <v>1</v>
       </c>
-      <c r="BB12" s="92">
-        <v>1</v>
-      </c>
-      <c r="BC12" s="93"/>
-      <c r="BD12" s="92">
-        <v>1</v>
-      </c>
-      <c r="BE12" s="93"/>
-      <c r="BF12" s="92">
-        <v>1</v>
-      </c>
-      <c r="BG12" s="93"/>
+      <c r="BB12" s="97">
+        <v>1</v>
+      </c>
+      <c r="BC12" s="98"/>
+      <c r="BD12" s="97">
+        <v>1</v>
+      </c>
+      <c r="BE12" s="98"/>
+      <c r="BF12" s="97">
+        <v>1</v>
+      </c>
+      <c r="BG12" s="98"/>
       <c r="BH12" s="27"/>
       <c r="BI12" s="27"/>
     </row>
     <row r="13" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="88"/>
+      <c r="A13" s="85"/>
       <c r="B13" s="2" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="94"/>
-      <c r="E13" s="95"/>
-      <c r="F13" s="94"/>
-      <c r="G13" s="95"/>
-      <c r="H13" s="94"/>
-      <c r="I13" s="95"/>
-      <c r="J13" s="94"/>
-      <c r="K13" s="95"/>
-      <c r="L13" s="94"/>
-      <c r="M13" s="95"/>
-      <c r="N13" s="94"/>
-      <c r="O13" s="95"/>
-      <c r="P13" s="94"/>
-      <c r="Q13" s="95"/>
-      <c r="R13" s="94"/>
-      <c r="S13" s="95"/>
-      <c r="T13" s="94"/>
-      <c r="U13" s="95"/>
-      <c r="V13" s="94"/>
-      <c r="W13" s="95"/>
-      <c r="X13" s="94"/>
-      <c r="Y13" s="95"/>
-      <c r="Z13" s="94"/>
-      <c r="AA13" s="95"/>
-      <c r="AB13" s="94"/>
-      <c r="AC13" s="95"/>
-      <c r="AD13" s="94"/>
-      <c r="AE13" s="95"/>
-      <c r="AF13" s="94"/>
-      <c r="AG13" s="95"/>
-      <c r="AH13" s="94"/>
-      <c r="AI13" s="95"/>
-      <c r="AJ13" s="94"/>
-      <c r="AK13" s="95"/>
-      <c r="AL13" s="94"/>
-      <c r="AM13" s="95"/>
+      <c r="D13" s="99"/>
+      <c r="E13" s="100"/>
+      <c r="F13" s="99"/>
+      <c r="G13" s="100"/>
+      <c r="H13" s="99"/>
+      <c r="I13" s="100"/>
+      <c r="J13" s="99"/>
+      <c r="K13" s="100"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="100"/>
+      <c r="N13" s="99"/>
+      <c r="O13" s="100"/>
+      <c r="P13" s="99"/>
+      <c r="Q13" s="100"/>
+      <c r="R13" s="99"/>
+      <c r="S13" s="100"/>
+      <c r="T13" s="99"/>
+      <c r="U13" s="100"/>
+      <c r="V13" s="99"/>
+      <c r="W13" s="100"/>
+      <c r="X13" s="99"/>
+      <c r="Y13" s="100"/>
+      <c r="Z13" s="99"/>
+      <c r="AA13" s="100"/>
+      <c r="AB13" s="99"/>
+      <c r="AC13" s="100"/>
+      <c r="AD13" s="99"/>
+      <c r="AE13" s="100"/>
+      <c r="AF13" s="99"/>
+      <c r="AG13" s="100"/>
+      <c r="AH13" s="99"/>
+      <c r="AI13" s="100"/>
+      <c r="AJ13" s="99"/>
+      <c r="AK13" s="100"/>
+      <c r="AL13" s="99"/>
+      <c r="AM13" s="100"/>
       <c r="AN13" s="33"/>
       <c r="AO13" s="33"/>
-      <c r="AP13" s="94"/>
-      <c r="AQ13" s="95"/>
-      <c r="AR13" s="94"/>
-      <c r="AS13" s="95"/>
-      <c r="AT13" s="94"/>
-      <c r="AU13" s="95"/>
-      <c r="AV13" s="94"/>
-      <c r="AW13" s="95"/>
-      <c r="AX13" s="94"/>
-      <c r="AY13" s="95"/>
+      <c r="AP13" s="99"/>
+      <c r="AQ13" s="100"/>
+      <c r="AR13" s="99"/>
+      <c r="AS13" s="100"/>
+      <c r="AT13" s="99"/>
+      <c r="AU13" s="100"/>
+      <c r="AV13" s="99"/>
+      <c r="AW13" s="100"/>
+      <c r="AX13" s="99"/>
+      <c r="AY13" s="100"/>
       <c r="AZ13" s="33"/>
       <c r="BA13" s="33"/>
-      <c r="BB13" s="94"/>
-      <c r="BC13" s="95"/>
-      <c r="BD13" s="94"/>
-      <c r="BE13" s="95"/>
-      <c r="BF13" s="94"/>
-      <c r="BG13" s="95"/>
+      <c r="BB13" s="99"/>
+      <c r="BC13" s="100"/>
+      <c r="BD13" s="99"/>
+      <c r="BE13" s="100"/>
+      <c r="BF13" s="99"/>
+      <c r="BG13" s="100"/>
       <c r="BH13" s="27"/>
       <c r="BI13" s="27"/>
     </row>
     <row r="14" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A14" s="88"/>
+      <c r="A14" s="85"/>
       <c r="B14" s="2" t="s">
         <v>22</v>
       </c>
@@ -7104,7 +7107,7 @@
       <c r="BI14" s="27"/>
     </row>
     <row r="15" spans="1:61" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="88"/>
+      <c r="A15" s="85"/>
       <c r="B15" s="2" t="s">
         <v>23</v>
       </c>
@@ -7175,7 +7178,7 @@
       <c r="BI15" s="27"/>
     </row>
     <row r="16" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A16" s="88"/>
+      <c r="A16" s="85"/>
       <c r="B16" s="2" t="s">
         <v>24</v>
       </c>
@@ -7246,7 +7249,7 @@
       <c r="BI16" s="27"/>
     </row>
     <row r="17" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A17" s="88"/>
+      <c r="A17" s="85"/>
       <c r="B17" s="2" t="s">
         <v>25</v>
       </c>
@@ -7313,7 +7316,7 @@
       <c r="BI17" s="27"/>
     </row>
     <row r="18" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="88" t="s">
+      <c r="A18" s="85" t="s">
         <v>28</v>
       </c>
       <c r="B18" s="6" t="s">
@@ -7444,7 +7447,7 @@
       <c r="BI18" s="27"/>
     </row>
     <row r="19" spans="1:61" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="88"/>
+      <c r="A19" s="85"/>
       <c r="B19" s="2" t="s">
         <v>31</v>
       </c>
@@ -7543,7 +7546,7 @@
       <c r="BI19" s="27"/>
     </row>
     <row r="20" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="88" t="s">
+      <c r="A20" s="85" t="s">
         <v>33</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -7658,7 +7661,7 @@
       <c r="BI20" s="27"/>
     </row>
     <row r="21" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A21" s="88"/>
+      <c r="A21" s="85"/>
       <c r="B21" s="2" t="s">
         <v>36</v>
       </c>
@@ -7747,14 +7750,13 @@
       <c r="BI21" s="27"/>
     </row>
     <row r="22" spans="1:61" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="88"/>
+      <c r="A22" s="85"/>
       <c r="B22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D22" s="18"/>
       <c r="E22" s="18"/>
       <c r="F22" s="33"/>
       <c r="G22" s="33"/>
@@ -7836,7 +7838,7 @@
       <c r="BI22" s="27"/>
     </row>
     <row r="23" spans="1:61" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="88"/>
+      <c r="A23" s="85"/>
       <c r="B23" s="6" t="s">
         <v>38</v>
       </c>
@@ -7903,7 +7905,7 @@
       <c r="BI23" s="27"/>
     </row>
     <row r="24" spans="1:61" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="88" t="s">
+      <c r="A24" s="85" t="s">
         <v>39</v>
       </c>
       <c r="B24" s="6" t="s">
@@ -7972,7 +7974,7 @@
       <c r="BI24" s="27"/>
     </row>
     <row r="25" spans="1:61" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="88"/>
+      <c r="A25" s="85"/>
       <c r="B25" s="2" t="s">
         <v>41</v>
       </c>
@@ -8039,7 +8041,7 @@
       <c r="BI25" s="27"/>
     </row>
     <row r="26" spans="1:61" ht="90" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="88"/>
+      <c r="A26" s="85"/>
       <c r="B26" s="6" t="s">
         <v>42</v>
       </c>
@@ -8106,10 +8108,10 @@
       <c r="BI26" s="27"/>
     </row>
     <row r="27" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="88" t="s">
+      <c r="A27" s="101" t="s">
         <v>43</v>
       </c>
-      <c r="B27" s="88"/>
+      <c r="B27" s="101"/>
       <c r="C27" s="17"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
@@ -8299,10 +8301,10 @@
       <c r="BI29" s="27"/>
     </row>
     <row r="30" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A30" s="98" t="s">
+      <c r="A30" s="95" t="s">
         <v>45</v>
       </c>
-      <c r="B30" s="98"/>
+      <c r="B30" s="95"/>
       <c r="C30" s="18"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
@@ -8314,10 +8316,10 @@
       <c r="K30" s="33"/>
       <c r="L30" s="33"/>
       <c r="M30" s="33"/>
-      <c r="N30" s="97">
+      <c r="N30" s="96">
         <v>2</v>
       </c>
-      <c r="O30" s="97"/>
+      <c r="O30" s="96"/>
       <c r="P30" s="33"/>
       <c r="Q30" s="33"/>
       <c r="R30" s="33"/>
@@ -8366,10 +8368,10 @@
       <c r="BI30" s="27"/>
     </row>
     <row r="31" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A31" s="98" t="s">
+      <c r="A31" s="95" t="s">
         <v>46</v>
       </c>
-      <c r="B31" s="98"/>
+      <c r="B31" s="95"/>
       <c r="C31" s="18"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
@@ -8433,10 +8435,10 @@
       <c r="BI31" s="27"/>
     </row>
     <row r="32" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A32" s="98" t="s">
+      <c r="A32" s="95" t="s">
         <v>47</v>
       </c>
-      <c r="B32" s="98"/>
+      <c r="B32" s="95"/>
       <c r="C32" s="18"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
@@ -8450,10 +8452,10 @@
       <c r="M32" s="33"/>
       <c r="N32" s="33"/>
       <c r="O32" s="33"/>
-      <c r="P32" s="97">
+      <c r="P32" s="96">
         <v>2</v>
       </c>
-      <c r="Q32" s="97"/>
+      <c r="Q32" s="96"/>
       <c r="R32" s="42"/>
       <c r="S32" s="42"/>
       <c r="T32" s="42"/>
@@ -8500,10 +8502,10 @@
       <c r="BI32" s="27"/>
     </row>
     <row r="33" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="98" t="s">
+      <c r="A33" s="95" t="s">
         <v>48</v>
       </c>
-      <c r="B33" s="98"/>
+      <c r="B33" s="95"/>
       <c r="C33" s="18"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
@@ -8517,10 +8519,10 @@
       <c r="M33" s="33"/>
       <c r="N33" s="33"/>
       <c r="O33" s="33"/>
-      <c r="P33" s="97">
-        <v>1</v>
-      </c>
-      <c r="Q33" s="97"/>
+      <c r="P33" s="96">
+        <v>1</v>
+      </c>
+      <c r="Q33" s="96"/>
       <c r="R33" s="42"/>
       <c r="S33" s="42"/>
       <c r="T33" s="42"/>
@@ -8567,10 +8569,10 @@
       <c r="BI33" s="27"/>
     </row>
     <row r="34" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="98" t="s">
+      <c r="A34" s="95" t="s">
         <v>49</v>
       </c>
-      <c r="B34" s="98"/>
+      <c r="B34" s="95"/>
       <c r="C34" s="18"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
@@ -8586,10 +8588,10 @@
       <c r="O34" s="33"/>
       <c r="P34" s="42"/>
       <c r="Q34" s="42"/>
-      <c r="R34" s="97">
-        <v>1</v>
-      </c>
-      <c r="S34" s="97"/>
+      <c r="R34" s="96">
+        <v>1</v>
+      </c>
+      <c r="S34" s="96"/>
       <c r="T34" s="42"/>
       <c r="U34" s="42"/>
       <c r="V34" s="33"/>
@@ -8634,10 +8636,10 @@
       <c r="BI34" s="27"/>
     </row>
     <row r="35" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="98" t="s">
+      <c r="A35" s="95" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="98"/>
+      <c r="B35" s="95"/>
       <c r="C35" s="18"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
@@ -8653,10 +8655,10 @@
       <c r="O35" s="33"/>
       <c r="P35" s="42"/>
       <c r="Q35" s="42"/>
-      <c r="R35" s="97">
+      <c r="R35" s="96">
         <v>2</v>
       </c>
-      <c r="S35" s="97"/>
+      <c r="S35" s="96"/>
       <c r="T35" s="42"/>
       <c r="U35" s="42"/>
       <c r="V35" s="33"/>
@@ -8701,10 +8703,10 @@
       <c r="BI35" s="27"/>
     </row>
     <row r="36" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="98" t="s">
+      <c r="A36" s="95" t="s">
         <v>51</v>
       </c>
-      <c r="B36" s="98"/>
+      <c r="B36" s="95"/>
       <c r="C36" s="18"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
@@ -8722,10 +8724,10 @@
       <c r="Q36" s="42"/>
       <c r="R36" s="33"/>
       <c r="S36" s="33"/>
-      <c r="T36" s="97">
+      <c r="T36" s="96">
         <v>2</v>
       </c>
-      <c r="U36" s="97"/>
+      <c r="U36" s="96"/>
       <c r="V36" s="33"/>
       <c r="W36" s="33"/>
       <c r="X36" s="33"/>
@@ -8768,10 +8770,10 @@
       <c r="BI36" s="27"/>
     </row>
     <row r="37" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="98" t="s">
+      <c r="A37" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="98"/>
+      <c r="B37" s="95"/>
       <c r="C37" s="18"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
@@ -8789,10 +8791,10 @@
       <c r="Q37" s="42"/>
       <c r="R37" s="33"/>
       <c r="S37" s="33"/>
-      <c r="T37" s="97">
+      <c r="T37" s="96">
         <v>2</v>
       </c>
-      <c r="U37" s="97"/>
+      <c r="U37" s="96"/>
       <c r="V37" s="33"/>
       <c r="W37" s="33"/>
       <c r="X37" s="33"/>
@@ -8835,10 +8837,10 @@
       <c r="BI37" s="27"/>
     </row>
     <row r="38" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A38" s="98" t="s">
+      <c r="A38" s="95" t="s">
         <v>53</v>
       </c>
-      <c r="B38" s="98"/>
+      <c r="B38" s="95"/>
       <c r="C38" s="18"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -8858,10 +8860,10 @@
       <c r="S38" s="33"/>
       <c r="T38" s="33"/>
       <c r="U38" s="33"/>
-      <c r="V38" s="97">
+      <c r="V38" s="96">
         <v>2</v>
       </c>
-      <c r="W38" s="97"/>
+      <c r="W38" s="96"/>
       <c r="X38" s="33"/>
       <c r="Y38" s="33"/>
       <c r="Z38" s="33"/>
@@ -8902,10 +8904,10 @@
       <c r="BI38" s="27"/>
     </row>
     <row r="39" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A39" s="98" t="s">
+      <c r="A39" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="B39" s="98"/>
+      <c r="B39" s="95"/>
       <c r="C39" s="18"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -8925,10 +8927,10 @@
       <c r="S39" s="33"/>
       <c r="T39" s="33"/>
       <c r="U39" s="33"/>
-      <c r="V39" s="97">
+      <c r="V39" s="96">
         <v>2</v>
       </c>
-      <c r="W39" s="97"/>
+      <c r="W39" s="96"/>
       <c r="X39" s="33"/>
       <c r="Y39" s="33"/>
       <c r="Z39" s="33"/>
@@ -8969,10 +8971,10 @@
       <c r="BI39" s="27"/>
     </row>
     <row r="40" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A40" s="98" t="s">
+      <c r="A40" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B40" s="98"/>
+      <c r="B40" s="95"/>
       <c r="C40" s="18"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
@@ -8994,10 +8996,10 @@
       <c r="U40" s="33"/>
       <c r="V40" s="33"/>
       <c r="W40" s="33"/>
-      <c r="X40" s="97">
+      <c r="X40" s="96">
         <v>2</v>
       </c>
-      <c r="Y40" s="97"/>
+      <c r="Y40" s="96"/>
       <c r="Z40" s="33"/>
       <c r="AA40" s="33"/>
       <c r="AB40" s="33"/>
@@ -9036,10 +9038,10 @@
       <c r="BI40" s="27"/>
     </row>
     <row r="41" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A41" s="98" t="s">
+      <c r="A41" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="98"/>
+      <c r="B41" s="95"/>
       <c r="C41" s="18"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
@@ -9061,10 +9063,10 @@
       <c r="U41" s="33"/>
       <c r="V41" s="33"/>
       <c r="W41" s="33"/>
-      <c r="X41" s="97">
+      <c r="X41" s="96">
         <v>2</v>
       </c>
-      <c r="Y41" s="97"/>
+      <c r="Y41" s="96"/>
       <c r="Z41" s="33"/>
       <c r="AA41" s="33"/>
       <c r="AB41" s="33"/>
@@ -9103,10 +9105,10 @@
       <c r="BI41" s="27"/>
     </row>
     <row r="42" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A42" s="98" t="s">
+      <c r="A42" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="B42" s="98"/>
+      <c r="B42" s="95"/>
       <c r="C42" s="18"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
@@ -9130,10 +9132,10 @@
       <c r="W42" s="33"/>
       <c r="X42" s="33"/>
       <c r="Y42" s="33"/>
-      <c r="Z42" s="97">
+      <c r="Z42" s="96">
         <v>2</v>
       </c>
-      <c r="AA42" s="97"/>
+      <c r="AA42" s="96"/>
       <c r="AB42" s="33"/>
       <c r="AC42" s="33"/>
       <c r="AD42" s="33"/>
@@ -9170,10 +9172,10 @@
       <c r="BI42" s="27"/>
     </row>
     <row r="43" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A43" s="98" t="s">
+      <c r="A43" s="95" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="98"/>
+      <c r="B43" s="95"/>
       <c r="C43" s="18"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -9197,10 +9199,10 @@
       <c r="W43" s="33"/>
       <c r="X43" s="33"/>
       <c r="Y43" s="33"/>
-      <c r="Z43" s="97">
+      <c r="Z43" s="96">
         <v>2</v>
       </c>
-      <c r="AA43" s="97"/>
+      <c r="AA43" s="96"/>
       <c r="AB43" s="33"/>
       <c r="AC43" s="33"/>
       <c r="AD43" s="33"/>
@@ -9237,10 +9239,10 @@
       <c r="BI43" s="27"/>
     </row>
     <row r="44" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A44" s="98" t="s">
+      <c r="A44" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="B44" s="98"/>
+      <c r="B44" s="95"/>
       <c r="C44" s="18"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -9290,14 +9292,14 @@
       <c r="AW44" s="33"/>
       <c r="AX44" s="33"/>
       <c r="AY44" s="33"/>
-      <c r="AZ44" s="97">
+      <c r="AZ44" s="96">
         <v>2</v>
       </c>
-      <c r="BA44" s="97"/>
-      <c r="BB44" s="97">
+      <c r="BA44" s="96"/>
+      <c r="BB44" s="96">
         <v>2</v>
       </c>
-      <c r="BC44" s="97"/>
+      <c r="BC44" s="96"/>
       <c r="BD44" s="33"/>
       <c r="BE44" s="33"/>
       <c r="BF44" s="33"/>
@@ -9306,10 +9308,10 @@
       <c r="BI44" s="27"/>
     </row>
     <row r="45" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A45" s="98" t="s">
+      <c r="A45" s="95" t="s">
         <v>60</v>
       </c>
-      <c r="B45" s="98"/>
+      <c r="B45" s="95"/>
       <c r="C45" s="18"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
@@ -9359,10 +9361,10 @@
       <c r="AW45" s="33"/>
       <c r="AX45" s="33"/>
       <c r="AY45" s="33"/>
-      <c r="AZ45" s="97">
+      <c r="AZ45" s="96">
         <v>2</v>
       </c>
-      <c r="BA45" s="97"/>
+      <c r="BA45" s="96"/>
       <c r="BB45" s="33"/>
       <c r="BC45" s="33"/>
       <c r="BD45" s="33"/>
@@ -9373,10 +9375,10 @@
       <c r="BI45" s="27"/>
     </row>
     <row r="46" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A46" s="98" t="s">
+      <c r="A46" s="95" t="s">
         <v>61</v>
       </c>
-      <c r="B46" s="98"/>
+      <c r="B46" s="95"/>
       <c r="C46" s="18"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
@@ -9428,10 +9430,10 @@
       <c r="AY46" s="33"/>
       <c r="AZ46" s="33"/>
       <c r="BA46" s="33"/>
-      <c r="BB46" s="97">
+      <c r="BB46" s="96">
         <v>2</v>
       </c>
-      <c r="BC46" s="97"/>
+      <c r="BC46" s="96"/>
       <c r="BD46" s="33"/>
       <c r="BE46" s="33"/>
       <c r="BF46" s="33"/>
@@ -9440,10 +9442,10 @@
       <c r="BI46" s="27"/>
     </row>
     <row r="47" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A47" s="98" t="s">
+      <c r="A47" s="95" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="98"/>
+      <c r="B47" s="95"/>
       <c r="C47" s="18"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
@@ -9497,20 +9499,20 @@
       <c r="BA47" s="33"/>
       <c r="BB47" s="33"/>
       <c r="BC47" s="33"/>
-      <c r="BD47" s="97">
+      <c r="BD47" s="96">
         <v>2</v>
       </c>
-      <c r="BE47" s="97"/>
+      <c r="BE47" s="96"/>
       <c r="BF47" s="33"/>
       <c r="BG47" s="33"/>
       <c r="BH47" s="27"/>
       <c r="BI47" s="27"/>
     </row>
     <row r="48" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A48" s="98" t="s">
+      <c r="A48" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="B48" s="98"/>
+      <c r="B48" s="95"/>
       <c r="C48" s="18"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -9564,20 +9566,20 @@
       <c r="BA48" s="33"/>
       <c r="BB48" s="33"/>
       <c r="BC48" s="33"/>
-      <c r="BD48" s="97">
+      <c r="BD48" s="96">
         <v>2</v>
       </c>
-      <c r="BE48" s="97"/>
+      <c r="BE48" s="96"/>
       <c r="BF48" s="33"/>
       <c r="BG48" s="33"/>
       <c r="BH48" s="27"/>
       <c r="BI48" s="27"/>
     </row>
     <row r="49" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A49" s="98" t="s">
+      <c r="A49" s="95" t="s">
         <v>64</v>
       </c>
-      <c r="B49" s="98"/>
+      <c r="B49" s="95"/>
       <c r="C49" s="18"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -9633,18 +9635,18 @@
       <c r="BC49" s="33"/>
       <c r="BD49" s="33"/>
       <c r="BE49" s="33"/>
-      <c r="BF49" s="97">
+      <c r="BF49" s="96">
         <v>2</v>
       </c>
-      <c r="BG49" s="97"/>
+      <c r="BG49" s="96"/>
       <c r="BH49" s="27"/>
       <c r="BI49" s="27"/>
     </row>
     <row r="50" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A50" s="98" t="s">
+      <c r="A50" s="95" t="s">
         <v>65</v>
       </c>
-      <c r="B50" s="98"/>
+      <c r="B50" s="95"/>
       <c r="C50" s="18"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
@@ -9700,18 +9702,18 @@
       <c r="BC50" s="33"/>
       <c r="BD50" s="33"/>
       <c r="BE50" s="33"/>
-      <c r="BF50" s="97">
+      <c r="BF50" s="96">
         <v>2</v>
       </c>
-      <c r="BG50" s="97"/>
+      <c r="BG50" s="96"/>
       <c r="BH50" s="27"/>
       <c r="BI50" s="27"/>
     </row>
     <row r="51" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A51" s="98" t="s">
+      <c r="A51" s="95" t="s">
         <v>66</v>
       </c>
-      <c r="B51" s="98"/>
+      <c r="B51" s="95"/>
       <c r="C51" s="18"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
@@ -9739,42 +9741,42 @@
       <c r="AA51" s="33"/>
       <c r="AB51" s="33"/>
       <c r="AC51" s="33"/>
-      <c r="AD51" s="97">
-        <v>1</v>
-      </c>
-      <c r="AE51" s="97"/>
-      <c r="AF51" s="97">
-        <v>1</v>
-      </c>
-      <c r="AG51" s="97"/>
-      <c r="AH51" s="97">
-        <v>1</v>
-      </c>
-      <c r="AI51" s="97"/>
-      <c r="AJ51" s="97">
-        <v>1</v>
-      </c>
-      <c r="AK51" s="97"/>
-      <c r="AL51" s="97">
-        <v>1</v>
-      </c>
-      <c r="AM51" s="97"/>
-      <c r="AN51" s="97">
-        <v>1</v>
-      </c>
-      <c r="AO51" s="97"/>
-      <c r="AP51" s="97">
-        <v>1</v>
-      </c>
-      <c r="AQ51" s="97"/>
-      <c r="AR51" s="97">
-        <v>1</v>
-      </c>
-      <c r="AS51" s="97"/>
-      <c r="AT51" s="97">
-        <v>1</v>
-      </c>
-      <c r="AU51" s="97"/>
+      <c r="AD51" s="96">
+        <v>1</v>
+      </c>
+      <c r="AE51" s="96"/>
+      <c r="AF51" s="96">
+        <v>1</v>
+      </c>
+      <c r="AG51" s="96"/>
+      <c r="AH51" s="96">
+        <v>1</v>
+      </c>
+      <c r="AI51" s="96"/>
+      <c r="AJ51" s="96">
+        <v>1</v>
+      </c>
+      <c r="AK51" s="96"/>
+      <c r="AL51" s="96">
+        <v>1</v>
+      </c>
+      <c r="AM51" s="96"/>
+      <c r="AN51" s="96">
+        <v>1</v>
+      </c>
+      <c r="AO51" s="96"/>
+      <c r="AP51" s="96">
+        <v>1</v>
+      </c>
+      <c r="AQ51" s="96"/>
+      <c r="AR51" s="96">
+        <v>1</v>
+      </c>
+      <c r="AS51" s="96"/>
+      <c r="AT51" s="96">
+        <v>1</v>
+      </c>
+      <c r="AU51" s="96"/>
       <c r="AV51" s="33"/>
       <c r="AW51" s="33"/>
       <c r="AX51" s="33"/>
@@ -9791,10 +9793,10 @@
       <c r="BI51" s="27"/>
     </row>
     <row r="52" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A52" s="98" t="s">
+      <c r="A52" s="95" t="s">
         <v>67</v>
       </c>
-      <c r="B52" s="98"/>
+      <c r="B52" s="95"/>
       <c r="C52" s="18"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
@@ -9828,10 +9830,10 @@
       <c r="AG52" s="33"/>
       <c r="AH52" s="33"/>
       <c r="AI52" s="33"/>
-      <c r="AJ52" s="97">
-        <v>1</v>
-      </c>
-      <c r="AK52" s="97"/>
+      <c r="AJ52" s="96">
+        <v>1</v>
+      </c>
+      <c r="AK52" s="96"/>
       <c r="AL52" s="33"/>
       <c r="AM52" s="33"/>
       <c r="AN52" s="33"/>
@@ -9858,10 +9860,10 @@
       <c r="BI52" s="27"/>
     </row>
     <row r="53" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A53" s="98" t="s">
+      <c r="A53" s="95" t="s">
         <v>68</v>
       </c>
-      <c r="B53" s="98"/>
+      <c r="B53" s="95"/>
       <c r="C53" s="18"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
@@ -9887,10 +9889,10 @@
       <c r="Y53" s="33"/>
       <c r="Z53" s="33"/>
       <c r="AA53" s="33"/>
-      <c r="AB53" s="97">
+      <c r="AB53" s="96">
         <v>2</v>
       </c>
-      <c r="AC53" s="97"/>
+      <c r="AC53" s="96"/>
       <c r="AD53" s="33"/>
       <c r="AE53" s="33"/>
       <c r="AF53" s="33"/>
@@ -9925,10 +9927,10 @@
       <c r="BI53" s="27"/>
     </row>
     <row r="54" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A54" s="98" t="s">
+      <c r="A54" s="95" t="s">
         <v>69</v>
       </c>
-      <c r="B54" s="98"/>
+      <c r="B54" s="95"/>
       <c r="C54" s="18"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
@@ -9954,10 +9956,10 @@
       <c r="Y54" s="33"/>
       <c r="Z54" s="33"/>
       <c r="AA54" s="33"/>
-      <c r="AB54" s="97">
-        <v>1</v>
-      </c>
-      <c r="AC54" s="97"/>
+      <c r="AB54" s="96">
+        <v>1</v>
+      </c>
+      <c r="AC54" s="96"/>
       <c r="AD54" s="33"/>
       <c r="AE54" s="33"/>
       <c r="AF54" s="33"/>
@@ -9992,10 +9994,10 @@
       <c r="BI54" s="27"/>
     </row>
     <row r="55" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A55" s="98" t="s">
+      <c r="A55" s="95" t="s">
         <v>70</v>
       </c>
-      <c r="B55" s="98"/>
+      <c r="B55" s="95"/>
       <c r="C55" s="18"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
@@ -10021,10 +10023,10 @@
       <c r="Y55" s="33"/>
       <c r="Z55" s="33"/>
       <c r="AA55" s="33"/>
-      <c r="AB55" s="97">
-        <v>1</v>
-      </c>
-      <c r="AC55" s="97"/>
+      <c r="AB55" s="96">
+        <v>1</v>
+      </c>
+      <c r="AC55" s="96"/>
       <c r="AD55" s="33"/>
       <c r="AE55" s="33"/>
       <c r="AF55" s="33"/>
@@ -10059,10 +10061,10 @@
       <c r="BI55" s="27"/>
     </row>
     <row r="56" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A56" s="98" t="s">
+      <c r="A56" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="B56" s="98"/>
+      <c r="B56" s="95"/>
       <c r="C56" s="18"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
@@ -10086,10 +10088,10 @@
       <c r="W56" s="33"/>
       <c r="X56" s="33"/>
       <c r="Y56" s="33"/>
-      <c r="Z56" s="97">
+      <c r="Z56" s="96">
         <v>2</v>
       </c>
-      <c r="AA56" s="97"/>
+      <c r="AA56" s="96"/>
       <c r="AB56" s="33"/>
       <c r="AC56" s="33"/>
       <c r="AD56" s="33"/>
@@ -10126,10 +10128,10 @@
       <c r="BI56" s="27"/>
     </row>
     <row r="57" spans="1:61" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="98" t="s">
+      <c r="A57" s="95" t="s">
         <v>71</v>
       </c>
-      <c r="B57" s="98"/>
+      <c r="B57" s="95"/>
       <c r="C57" s="18"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
@@ -10153,10 +10155,10 @@
       <c r="W57" s="33"/>
       <c r="X57" s="33"/>
       <c r="Y57" s="33"/>
-      <c r="Z57" s="97">
+      <c r="Z57" s="96">
         <v>2</v>
       </c>
-      <c r="AA57" s="97"/>
+      <c r="AA57" s="96"/>
       <c r="AB57" s="33"/>
       <c r="AC57" s="33"/>
       <c r="AD57" s="33"/>
@@ -10193,10 +10195,10 @@
       <c r="BI57" s="27"/>
     </row>
     <row r="58" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A58" s="98" t="s">
+      <c r="A58" s="95" t="s">
         <v>72</v>
       </c>
-      <c r="B58" s="98"/>
+      <c r="B58" s="95"/>
       <c r="C58" s="18"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
@@ -10224,10 +10226,10 @@
       <c r="AA58" s="33"/>
       <c r="AB58" s="33"/>
       <c r="AC58" s="33"/>
-      <c r="AD58" s="97">
-        <v>1</v>
-      </c>
-      <c r="AE58" s="97"/>
+      <c r="AD58" s="96">
+        <v>1</v>
+      </c>
+      <c r="AE58" s="96"/>
       <c r="AF58" s="33"/>
       <c r="AG58" s="33"/>
       <c r="AH58" s="33"/>
@@ -10260,10 +10262,10 @@
       <c r="BI58" s="27"/>
     </row>
     <row r="59" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A59" s="98" t="s">
+      <c r="A59" s="95" t="s">
         <v>52</v>
       </c>
-      <c r="B59" s="98"/>
+      <c r="B59" s="95"/>
       <c r="C59" s="18"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
@@ -10293,10 +10295,10 @@
       <c r="AC59" s="33"/>
       <c r="AD59" s="33"/>
       <c r="AE59" s="33"/>
-      <c r="AF59" s="97">
-        <v>1</v>
-      </c>
-      <c r="AG59" s="97"/>
+      <c r="AF59" s="96">
+        <v>1</v>
+      </c>
+      <c r="AG59" s="96"/>
       <c r="AH59" s="33"/>
       <c r="AI59" s="33"/>
       <c r="AJ59" s="33"/>
@@ -10327,10 +10329,10 @@
       <c r="BI59" s="27"/>
     </row>
     <row r="60" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A60" s="98" t="s">
+      <c r="A60" s="95" t="s">
         <v>73</v>
       </c>
-      <c r="B60" s="98"/>
+      <c r="B60" s="95"/>
       <c r="C60" s="18"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
@@ -10362,10 +10364,10 @@
       <c r="AE60" s="33"/>
       <c r="AF60" s="33"/>
       <c r="AG60" s="33"/>
-      <c r="AH60" s="97">
-        <v>1</v>
-      </c>
-      <c r="AI60" s="97"/>
+      <c r="AH60" s="96">
+        <v>1</v>
+      </c>
+      <c r="AI60" s="96"/>
       <c r="AJ60" s="33"/>
       <c r="AK60" s="33"/>
       <c r="AL60" s="33"/>
@@ -10394,10 +10396,10 @@
       <c r="BI60" s="27"/>
     </row>
     <row r="61" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A61" s="98" t="s">
+      <c r="A61" s="95" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="98"/>
+      <c r="B61" s="95"/>
       <c r="C61" s="18"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
@@ -10433,10 +10435,10 @@
       <c r="AI61" s="33"/>
       <c r="AJ61" s="33"/>
       <c r="AK61" s="33"/>
-      <c r="AL61" s="97">
-        <v>1</v>
-      </c>
-      <c r="AM61" s="97"/>
+      <c r="AL61" s="96">
+        <v>1</v>
+      </c>
+      <c r="AM61" s="96"/>
       <c r="AN61" s="33"/>
       <c r="AO61" s="33"/>
       <c r="AP61" s="33"/>
@@ -10461,10 +10463,10 @@
       <c r="BI61" s="27"/>
     </row>
     <row r="62" spans="1:61" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="98" t="s">
+      <c r="A62" s="95" t="s">
         <v>75</v>
       </c>
-      <c r="B62" s="98"/>
+      <c r="B62" s="95"/>
       <c r="C62" s="18"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
@@ -10500,10 +10502,10 @@
       <c r="AI62" s="33"/>
       <c r="AJ62" s="33"/>
       <c r="AK62" s="33"/>
-      <c r="AL62" s="97">
-        <v>1</v>
-      </c>
-      <c r="AM62" s="97"/>
+      <c r="AL62" s="96">
+        <v>1</v>
+      </c>
+      <c r="AM62" s="96"/>
       <c r="AN62" s="33"/>
       <c r="AO62" s="33"/>
       <c r="AP62" s="33"/>
@@ -10528,10 +10530,10 @@
       <c r="BI62" s="27"/>
     </row>
     <row r="63" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A63" s="98" t="s">
+      <c r="A63" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="B63" s="98"/>
+      <c r="B63" s="95"/>
       <c r="C63" s="18"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
@@ -10569,10 +10571,10 @@
       <c r="AK63" s="35"/>
       <c r="AL63" s="35"/>
       <c r="AM63" s="35"/>
-      <c r="AN63" s="97">
-        <v>1</v>
-      </c>
-      <c r="AO63" s="97"/>
+      <c r="AN63" s="96">
+        <v>1</v>
+      </c>
+      <c r="AO63" s="96"/>
       <c r="AP63" s="33"/>
       <c r="AQ63" s="33"/>
       <c r="AR63" s="33"/>
@@ -10595,10 +10597,10 @@
       <c r="BI63" s="27"/>
     </row>
     <row r="64" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A64" s="98" t="s">
+      <c r="A64" s="95" t="s">
         <v>77</v>
       </c>
-      <c r="B64" s="98"/>
+      <c r="B64" s="95"/>
       <c r="C64" s="18"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
@@ -10636,10 +10638,10 @@
       <c r="AK64" s="35"/>
       <c r="AL64" s="35"/>
       <c r="AM64" s="35"/>
-      <c r="AN64" s="97">
-        <v>1</v>
-      </c>
-      <c r="AO64" s="97"/>
+      <c r="AN64" s="96">
+        <v>1</v>
+      </c>
+      <c r="AO64" s="96"/>
       <c r="AP64" s="33"/>
       <c r="AQ64" s="33"/>
       <c r="AR64" s="33"/>
@@ -10662,10 +10664,10 @@
       <c r="BI64" s="27"/>
     </row>
     <row r="65" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A65" s="98" t="s">
+      <c r="A65" s="95" t="s">
         <v>0</v>
       </c>
-      <c r="B65" s="98"/>
+      <c r="B65" s="95"/>
       <c r="C65" s="18"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
@@ -10705,10 +10707,10 @@
       <c r="AM65" s="35"/>
       <c r="AN65" s="33"/>
       <c r="AO65" s="33"/>
-      <c r="AP65" s="97">
-        <v>1</v>
-      </c>
-      <c r="AQ65" s="97"/>
+      <c r="AP65" s="96">
+        <v>1</v>
+      </c>
+      <c r="AQ65" s="96"/>
       <c r="AR65" s="33"/>
       <c r="AS65" s="33"/>
       <c r="AT65" s="33"/>
@@ -10729,10 +10731,10 @@
       <c r="BI65" s="27"/>
     </row>
     <row r="66" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A66" s="98" t="s">
+      <c r="A66" s="95" t="s">
         <v>78</v>
       </c>
-      <c r="B66" s="98"/>
+      <c r="B66" s="95"/>
       <c r="C66" s="18"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
@@ -10772,10 +10774,10 @@
       <c r="AM66" s="35"/>
       <c r="AN66" s="33"/>
       <c r="AO66" s="33"/>
-      <c r="AP66" s="97">
-        <v>1</v>
-      </c>
-      <c r="AQ66" s="97"/>
+      <c r="AP66" s="96">
+        <v>1</v>
+      </c>
+      <c r="AQ66" s="96"/>
       <c r="AR66" s="33"/>
       <c r="AS66" s="33"/>
       <c r="AT66" s="33"/>
@@ -10796,10 +10798,10 @@
       <c r="BI66" s="27"/>
     </row>
     <row r="67" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A67" s="98" t="s">
+      <c r="A67" s="95" t="s">
         <v>79</v>
       </c>
-      <c r="B67" s="98"/>
+      <c r="B67" s="95"/>
       <c r="C67" s="18"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
@@ -10843,10 +10845,10 @@
       <c r="AQ67" s="33"/>
       <c r="AR67" s="33"/>
       <c r="AS67" s="33"/>
-      <c r="AT67" s="97">
+      <c r="AT67" s="96">
         <v>3</v>
       </c>
-      <c r="AU67" s="97"/>
+      <c r="AU67" s="96"/>
       <c r="AV67" s="33"/>
       <c r="AW67" s="33"/>
       <c r="AX67" s="33"/>
@@ -10863,10 +10865,10 @@
       <c r="BI67" s="27"/>
     </row>
     <row r="68" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A68" s="98" t="s">
+      <c r="A68" s="95" t="s">
         <v>80</v>
       </c>
-      <c r="B68" s="98"/>
+      <c r="B68" s="95"/>
       <c r="C68" s="18"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
@@ -10910,10 +10912,10 @@
       <c r="AQ68" s="33"/>
       <c r="AR68" s="33"/>
       <c r="AS68" s="33"/>
-      <c r="AT68" s="97">
+      <c r="AT68" s="96">
         <v>2</v>
       </c>
-      <c r="AU68" s="97"/>
+      <c r="AU68" s="96"/>
       <c r="AV68" s="33"/>
       <c r="AW68" s="33"/>
       <c r="AX68" s="33"/>
@@ -10930,10 +10932,10 @@
       <c r="BI68" s="27"/>
     </row>
     <row r="69" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A69" s="98" t="s">
+      <c r="A69" s="95" t="s">
         <v>81</v>
       </c>
-      <c r="B69" s="98"/>
+      <c r="B69" s="95"/>
       <c r="C69" s="18"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
@@ -10981,10 +10983,10 @@
       <c r="AU69" s="33"/>
       <c r="AV69" s="33"/>
       <c r="AW69" s="33"/>
-      <c r="AX69" s="97">
+      <c r="AX69" s="96">
         <v>2</v>
       </c>
-      <c r="AY69" s="97"/>
+      <c r="AY69" s="96"/>
       <c r="AZ69" s="33"/>
       <c r="BA69" s="33"/>
       <c r="BB69" s="33"/>
@@ -10997,10 +10999,10 @@
       <c r="BI69" s="27"/>
     </row>
     <row r="70" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A70" s="98" t="s">
+      <c r="A70" s="95" t="s">
         <v>82</v>
       </c>
-      <c r="B70" s="98"/>
+      <c r="B70" s="95"/>
       <c r="C70" s="18"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
@@ -11048,10 +11050,10 @@
       <c r="AU70" s="33"/>
       <c r="AV70" s="33"/>
       <c r="AW70" s="33"/>
-      <c r="AX70" s="97">
+      <c r="AX70" s="96">
         <v>2</v>
       </c>
-      <c r="AY70" s="97"/>
+      <c r="AY70" s="96"/>
       <c r="AZ70" s="33"/>
       <c r="BA70" s="33"/>
       <c r="BB70" s="33"/>
@@ -11064,10 +11066,10 @@
       <c r="BI70" s="27"/>
     </row>
     <row r="71" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A71" s="98" t="s">
+      <c r="A71" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="B71" s="98"/>
+      <c r="B71" s="95"/>
       <c r="C71" s="18"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
@@ -11115,10 +11117,10 @@
       <c r="AU71" s="33"/>
       <c r="AV71" s="33"/>
       <c r="AW71" s="33"/>
-      <c r="AX71" s="97">
+      <c r="AX71" s="96">
         <v>2</v>
       </c>
-      <c r="AY71" s="97"/>
+      <c r="AY71" s="96"/>
       <c r="AZ71" s="33"/>
       <c r="BA71" s="33"/>
       <c r="BB71" s="33"/>
@@ -11131,10 +11133,10 @@
       <c r="BI71" s="27"/>
     </row>
     <row r="72" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A72" s="98" t="s">
+      <c r="A72" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="B72" s="98"/>
+      <c r="B72" s="95"/>
       <c r="C72" s="18"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
@@ -11182,10 +11184,10 @@
       <c r="AU72" s="33"/>
       <c r="AV72" s="33"/>
       <c r="AW72" s="33"/>
-      <c r="AX72" s="97">
+      <c r="AX72" s="96">
         <v>2</v>
       </c>
-      <c r="AY72" s="97"/>
+      <c r="AY72" s="96"/>
       <c r="AZ72" s="33"/>
       <c r="BA72" s="33"/>
       <c r="BB72" s="33"/>
@@ -11198,10 +11200,10 @@
       <c r="BI72" s="27"/>
     </row>
     <row r="73" spans="1:61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="98" t="s">
+      <c r="A73" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="B73" s="98"/>
+      <c r="B73" s="95"/>
       <c r="C73" s="18"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
@@ -11247,10 +11249,10 @@
       <c r="AS73" s="33"/>
       <c r="AT73" s="33"/>
       <c r="AU73" s="33"/>
-      <c r="AV73" s="97" t="s">
+      <c r="AV73" s="96" t="s">
         <v>167</v>
       </c>
-      <c r="AW73" s="97"/>
+      <c r="AW73" s="96"/>
       <c r="AX73" s="33"/>
       <c r="AY73" s="33"/>
       <c r="AZ73" s="33"/>
@@ -11265,10 +11267,10 @@
       <c r="BI73" s="27"/>
     </row>
     <row r="74" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A74" s="98" t="s">
+      <c r="A74" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="B74" s="98"/>
+      <c r="B74" s="95"/>
       <c r="C74" s="18"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
@@ -11314,8 +11316,8 @@
       <c r="AS74" s="33"/>
       <c r="AT74" s="33"/>
       <c r="AU74" s="33"/>
-      <c r="AV74" s="97"/>
-      <c r="AW74" s="97"/>
+      <c r="AV74" s="96"/>
+      <c r="AW74" s="96"/>
       <c r="AX74" s="33"/>
       <c r="AY74" s="33"/>
       <c r="AZ74" s="33"/>
@@ -11330,10 +11332,10 @@
       <c r="BI74" s="27"/>
     </row>
     <row r="75" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A75" s="98" t="s">
+      <c r="A75" s="95" t="s">
         <v>86</v>
       </c>
-      <c r="B75" s="98"/>
+      <c r="B75" s="95"/>
       <c r="C75" s="18"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
@@ -11379,8 +11381,8 @@
       <c r="AS75" s="33"/>
       <c r="AT75" s="33"/>
       <c r="AU75" s="33"/>
-      <c r="AV75" s="97"/>
-      <c r="AW75" s="97"/>
+      <c r="AV75" s="96"/>
+      <c r="AW75" s="96"/>
       <c r="AX75" s="33"/>
       <c r="AY75" s="33"/>
       <c r="AZ75" s="33"/>
@@ -11395,10 +11397,10 @@
       <c r="BI75" s="27"/>
     </row>
     <row r="76" spans="1:61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="98" t="s">
+      <c r="A76" s="95" t="s">
         <v>87</v>
       </c>
-      <c r="B76" s="98"/>
+      <c r="B76" s="95"/>
       <c r="C76" s="18"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
@@ -11444,8 +11446,8 @@
       <c r="AS76" s="33"/>
       <c r="AT76" s="33"/>
       <c r="AU76" s="33"/>
-      <c r="AV76" s="97"/>
-      <c r="AW76" s="97"/>
+      <c r="AV76" s="96"/>
+      <c r="AW76" s="96"/>
       <c r="AX76" s="33"/>
       <c r="AY76" s="33"/>
       <c r="AZ76" s="33"/>
@@ -11460,10 +11462,10 @@
       <c r="BI76" s="27"/>
     </row>
     <row r="77" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A77" s="98" t="s">
+      <c r="A77" s="95" t="s">
         <v>168</v>
       </c>
-      <c r="B77" s="98"/>
+      <c r="B77" s="95"/>
       <c r="C77" s="18"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
@@ -11509,8 +11511,8 @@
       <c r="AS77" s="33"/>
       <c r="AT77" s="33"/>
       <c r="AU77" s="33"/>
-      <c r="AV77" s="97"/>
-      <c r="AW77" s="97"/>
+      <c r="AV77" s="96"/>
+      <c r="AW77" s="96"/>
       <c r="AX77" s="33"/>
       <c r="AY77" s="33"/>
       <c r="AZ77" s="33"/>
@@ -11525,10 +11527,10 @@
       <c r="BI77" s="27"/>
     </row>
     <row r="78" spans="1:61" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A78" s="98" t="s">
+      <c r="A78" s="95" t="s">
         <v>88</v>
       </c>
-      <c r="B78" s="98"/>
+      <c r="B78" s="95"/>
       <c r="C78" s="18"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
@@ -11574,8 +11576,8 @@
       <c r="AS78" s="33"/>
       <c r="AT78" s="33"/>
       <c r="AU78" s="33"/>
-      <c r="AV78" s="97"/>
-      <c r="AW78" s="97"/>
+      <c r="AV78" s="96"/>
+      <c r="AW78" s="96"/>
       <c r="AX78" s="33"/>
       <c r="AY78" s="33"/>
       <c r="AZ78" s="33"/>
@@ -11785,7 +11787,7 @@
       <c r="BI81" s="27"/>
     </row>
     <row r="82" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A82" s="90" t="s">
+      <c r="A82" s="89" t="s">
         <v>119</v>
       </c>
       <c r="B82" s="46" t="s">
@@ -11854,7 +11856,7 @@
       <c r="BI82" s="27"/>
     </row>
     <row r="83" spans="1:61" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A83" s="90"/>
+      <c r="A83" s="89"/>
       <c r="B83" s="46">
         <v>2170</v>
       </c>
@@ -11921,7 +11923,7 @@
       <c r="BI83" s="27"/>
     </row>
     <row r="84" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A84" s="99" t="s">
+      <c r="A84" s="92" t="s">
         <v>118</v>
       </c>
       <c r="B84" s="46">
@@ -11990,7 +11992,7 @@
       <c r="BI84" s="27"/>
     </row>
     <row r="85" spans="1:61" x14ac:dyDescent="0.3">
-      <c r="A85" s="99"/>
+      <c r="A85" s="92"/>
       <c r="B85" s="46">
         <v>34</v>
       </c>
@@ -12448,6 +12450,138 @@
     </row>
   </sheetData>
   <mergeCells count="156">
+    <mergeCell ref="P12:Q13"/>
+    <mergeCell ref="R12:S13"/>
+    <mergeCell ref="AV12:AW13"/>
+    <mergeCell ref="T12:U13"/>
+    <mergeCell ref="V12:W13"/>
+    <mergeCell ref="X12:Y13"/>
+    <mergeCell ref="Z12:AA13"/>
+    <mergeCell ref="BD12:BE13"/>
+    <mergeCell ref="BF12:BG13"/>
+    <mergeCell ref="AL12:AM13"/>
+    <mergeCell ref="AP12:AQ13"/>
+    <mergeCell ref="AR12:AS13"/>
+    <mergeCell ref="AT12:AU13"/>
+    <mergeCell ref="AB12:AC13"/>
+    <mergeCell ref="AD12:AE13"/>
+    <mergeCell ref="AF12:AG13"/>
+    <mergeCell ref="AH12:AI13"/>
+    <mergeCell ref="AJ12:AK13"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="AZ1:BA1"/>
+    <mergeCell ref="BB1:BC1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="AN1:AO1"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AR1:AS1"/>
+    <mergeCell ref="AT1:AU1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AX1:AY1"/>
+    <mergeCell ref="AD1:AE1"/>
+    <mergeCell ref="AF1:AG1"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AJ1:AK1"/>
+    <mergeCell ref="AL1:AM1"/>
+    <mergeCell ref="AX12:AY13"/>
+    <mergeCell ref="BB12:BC13"/>
+    <mergeCell ref="D12:E13"/>
+    <mergeCell ref="F12:G13"/>
+    <mergeCell ref="H12:I13"/>
+    <mergeCell ref="J12:K13"/>
+    <mergeCell ref="L12:M13"/>
+    <mergeCell ref="N12:O13"/>
+    <mergeCell ref="R35:S35"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="T36:U36"/>
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="T37:U37"/>
+    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="P32:Q32"/>
+    <mergeCell ref="A33:B33"/>
+    <mergeCell ref="P33:Q33"/>
+    <mergeCell ref="A34:B34"/>
+    <mergeCell ref="R34:S34"/>
+    <mergeCell ref="X41:Y41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="Z42:AA42"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="Z43:AA43"/>
+    <mergeCell ref="A38:B38"/>
+    <mergeCell ref="V38:W38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="V39:W39"/>
+    <mergeCell ref="A40:B40"/>
+    <mergeCell ref="X40:Y40"/>
+    <mergeCell ref="BD47:BE47"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="BD48:BE48"/>
+    <mergeCell ref="A49:B49"/>
+    <mergeCell ref="BF49:BG49"/>
+    <mergeCell ref="A44:B44"/>
+    <mergeCell ref="AZ44:BA44"/>
+    <mergeCell ref="BB44:BC44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="AZ45:BA45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="BB46:BC46"/>
+    <mergeCell ref="BF50:BG50"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="AD51:AE51"/>
+    <mergeCell ref="AF51:AG51"/>
+    <mergeCell ref="AH51:AI51"/>
+    <mergeCell ref="AJ51:AK51"/>
+    <mergeCell ref="AL51:AM51"/>
+    <mergeCell ref="AN51:AO51"/>
+    <mergeCell ref="AP51:AQ51"/>
+    <mergeCell ref="AB54:AC54"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="AB55:AC55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="Z56:AA56"/>
+    <mergeCell ref="AR51:AS51"/>
+    <mergeCell ref="AT51:AU51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="AJ52:AK52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="AB53:AC53"/>
+    <mergeCell ref="AH60:AI60"/>
+    <mergeCell ref="A61:B61"/>
+    <mergeCell ref="AL61:AM61"/>
+    <mergeCell ref="A62:B62"/>
+    <mergeCell ref="AL62:AM62"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="Z57:AA57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="AD58:AE58"/>
+    <mergeCell ref="A59:B59"/>
+    <mergeCell ref="AF59:AG59"/>
+    <mergeCell ref="AP66:AQ66"/>
+    <mergeCell ref="A67:B67"/>
+    <mergeCell ref="AT67:AU67"/>
+    <mergeCell ref="A68:B68"/>
+    <mergeCell ref="AT68:AU68"/>
+    <mergeCell ref="A63:B63"/>
+    <mergeCell ref="AN63:AO63"/>
+    <mergeCell ref="A64:B64"/>
+    <mergeCell ref="AN64:AO64"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="AP65:AQ65"/>
+    <mergeCell ref="AX72:AY72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="AV73:AW78"/>
+    <mergeCell ref="A74:B74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A77:B77"/>
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A69:B69"/>
+    <mergeCell ref="AX69:AY69"/>
+    <mergeCell ref="A70:B70"/>
+    <mergeCell ref="AX70:AY70"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="AX71:AY71"/>
     <mergeCell ref="A82:A83"/>
     <mergeCell ref="A84:A85"/>
     <mergeCell ref="N1:O1"/>
@@ -12471,139 +12605,7 @@
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="A10:A11"/>
     <mergeCell ref="A12:A17"/>
-    <mergeCell ref="AX72:AY72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="AV73:AW78"/>
-    <mergeCell ref="A74:B74"/>
-    <mergeCell ref="A75:B75"/>
-    <mergeCell ref="A76:B76"/>
-    <mergeCell ref="A77:B77"/>
-    <mergeCell ref="A78:B78"/>
-    <mergeCell ref="A69:B69"/>
-    <mergeCell ref="AX69:AY69"/>
-    <mergeCell ref="A70:B70"/>
-    <mergeCell ref="AX70:AY70"/>
-    <mergeCell ref="A71:B71"/>
-    <mergeCell ref="AX71:AY71"/>
-    <mergeCell ref="AP66:AQ66"/>
-    <mergeCell ref="A67:B67"/>
-    <mergeCell ref="AT67:AU67"/>
-    <mergeCell ref="A68:B68"/>
-    <mergeCell ref="AT68:AU68"/>
-    <mergeCell ref="A63:B63"/>
-    <mergeCell ref="AN63:AO63"/>
-    <mergeCell ref="A64:B64"/>
-    <mergeCell ref="AN64:AO64"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="AP65:AQ65"/>
-    <mergeCell ref="AH60:AI60"/>
-    <mergeCell ref="A61:B61"/>
-    <mergeCell ref="AL61:AM61"/>
-    <mergeCell ref="A62:B62"/>
-    <mergeCell ref="AL62:AM62"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="Z57:AA57"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="AD58:AE58"/>
-    <mergeCell ref="A59:B59"/>
-    <mergeCell ref="AF59:AG59"/>
-    <mergeCell ref="AB54:AC54"/>
-    <mergeCell ref="A55:B55"/>
-    <mergeCell ref="AB55:AC55"/>
-    <mergeCell ref="A56:B56"/>
-    <mergeCell ref="Z56:AA56"/>
-    <mergeCell ref="AR51:AS51"/>
-    <mergeCell ref="AT51:AU51"/>
-    <mergeCell ref="A52:B52"/>
-    <mergeCell ref="AJ52:AK52"/>
-    <mergeCell ref="A53:B53"/>
-    <mergeCell ref="AB53:AC53"/>
-    <mergeCell ref="BF50:BG50"/>
-    <mergeCell ref="A51:B51"/>
-    <mergeCell ref="AD51:AE51"/>
-    <mergeCell ref="AF51:AG51"/>
-    <mergeCell ref="AH51:AI51"/>
-    <mergeCell ref="AJ51:AK51"/>
-    <mergeCell ref="AL51:AM51"/>
-    <mergeCell ref="AN51:AO51"/>
-    <mergeCell ref="AP51:AQ51"/>
-    <mergeCell ref="BD47:BE47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="BD48:BE48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="BF49:BG49"/>
-    <mergeCell ref="A44:B44"/>
-    <mergeCell ref="AZ44:BA44"/>
-    <mergeCell ref="BB44:BC44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="AZ45:BA45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="BB46:BC46"/>
-    <mergeCell ref="X41:Y41"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="Z42:AA42"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="Z43:AA43"/>
-    <mergeCell ref="A38:B38"/>
-    <mergeCell ref="V38:W38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="V39:W39"/>
-    <mergeCell ref="A40:B40"/>
-    <mergeCell ref="X40:Y40"/>
-    <mergeCell ref="R35:S35"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="T36:U36"/>
-    <mergeCell ref="A37:B37"/>
-    <mergeCell ref="T37:U37"/>
-    <mergeCell ref="A32:B32"/>
-    <mergeCell ref="P32:Q32"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="P33:Q33"/>
-    <mergeCell ref="A34:B34"/>
-    <mergeCell ref="R34:S34"/>
     <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="AZ1:BA1"/>
-    <mergeCell ref="BB1:BC1"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="AN1:AO1"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AR1:AS1"/>
-    <mergeCell ref="AT1:AU1"/>
-    <mergeCell ref="AV1:AW1"/>
-    <mergeCell ref="AX1:AY1"/>
-    <mergeCell ref="AD1:AE1"/>
-    <mergeCell ref="AF1:AG1"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AJ1:AK1"/>
-    <mergeCell ref="AL1:AM1"/>
-    <mergeCell ref="AX12:AY13"/>
-    <mergeCell ref="BB12:BC13"/>
-    <mergeCell ref="BD12:BE13"/>
-    <mergeCell ref="BF12:BG13"/>
-    <mergeCell ref="AL12:AM13"/>
-    <mergeCell ref="AP12:AQ13"/>
-    <mergeCell ref="AR12:AS13"/>
-    <mergeCell ref="AT12:AU13"/>
-    <mergeCell ref="AB12:AC13"/>
-    <mergeCell ref="AD12:AE13"/>
-    <mergeCell ref="AF12:AG13"/>
-    <mergeCell ref="AH12:AI13"/>
-    <mergeCell ref="AJ12:AK13"/>
-    <mergeCell ref="D12:E13"/>
-    <mergeCell ref="F12:G13"/>
-    <mergeCell ref="H12:I13"/>
-    <mergeCell ref="J12:K13"/>
-    <mergeCell ref="L12:M13"/>
-    <mergeCell ref="N12:O13"/>
-    <mergeCell ref="P12:Q13"/>
-    <mergeCell ref="R12:S13"/>
-    <mergeCell ref="AV12:AW13"/>
-    <mergeCell ref="T12:U13"/>
-    <mergeCell ref="V12:W13"/>
-    <mergeCell ref="X12:Y13"/>
-    <mergeCell ref="Z12:AA13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>